<commit_message>
added smiles string to excel sheet added a few warning qt pop ups updated all example problems to incorporate smiles in excel sheet
</commit_message>
<xml_diff>
--- a/exampleProblems/Problem74/Problem74.xlsx
+++ b/exampleProblems/Problem74/Problem74.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/Problem74/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9E928023-5053-F245-B341-BC75B97C5C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5A73A5B-8594-F748-9AD2-C9A859F0F93A}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{9E928023-5053-F245-B341-BC75B97C5C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C7C986-3406-41BF-A24C-67CE759F40EB}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="500" windowWidth="27980" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7275" yWindow="990" windowWidth="20295" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>smiles</t>
+  </si>
+  <si>
+    <t>CC1(C)OC(C(O)CO)C(C(O)CO)O1</t>
   </si>
 </sst>
 </file>
@@ -629,28 +635,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -662,17 +675,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17">
+    <row r="1" spans="1:9" ht="16.5">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -699,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17">
+    <row r="2" spans="1:9" ht="16.5">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -728,7 +741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:9" ht="16.5">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -757,7 +770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17">
+    <row r="4" spans="1:9" ht="16.5">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -786,7 +799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17">
+    <row r="5" spans="1:9" ht="16.5">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -815,7 +828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17">
+    <row r="6" spans="1:9" ht="16.5">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -844,7 +857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17">
+    <row r="7" spans="1:9" ht="16.5">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -873,7 +886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17">
+    <row r="8" spans="1:9" ht="16.5">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -927,9 +940,9 @@
       <selection activeCell="K7" sqref="A7:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="17">
+    <row r="1" spans="1:13" ht="16.5">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>18</v>
@@ -962,7 +975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17">
+    <row r="2" spans="1:13" ht="16.5">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -994,7 +1007,7 @@
       <c r="K2" s="11"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="17">
+    <row r="3" spans="1:13" ht="16.5">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1026,7 +1039,7 @@
       <c r="K3" s="11"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="17">
+    <row r="4" spans="1:13" ht="16.5">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1058,7 +1071,7 @@
       <c r="K4" s="11"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="17">
+    <row r="5" spans="1:13" ht="16.5">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1090,7 +1103,7 @@
       <c r="K5" s="11"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="17">
+    <row r="6" spans="1:13" ht="16.5">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1200,9 +1213,9 @@
       <selection activeCell="K14" sqref="A1:K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="17">
+    <row r="1" spans="1:22" ht="16.5">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>18</v>
@@ -1246,7 +1259,7 @@
       <c r="U1" s="3"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" ht="17">
+    <row r="2" spans="1:22" ht="16.5">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1279,7 +1292,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:22" ht="17">
+    <row r="3" spans="1:22" ht="16.5">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1312,7 +1325,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22" ht="17">
+    <row r="4" spans="1:22" ht="16.5">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1345,7 +1358,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="17">
+    <row r="5" spans="1:22" ht="16.5">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1378,7 +1391,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="1:22" ht="17">
+    <row r="6" spans="1:22" ht="16.5">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1411,7 +1424,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:22" ht="17">
+    <row r="7" spans="1:22" ht="16.5">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1444,7 +1457,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" spans="1:22" ht="17">
+    <row r="8" spans="1:22" ht="16.5">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1477,7 +1490,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" ht="17">
+    <row r="9" spans="1:22" ht="16.5">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1510,7 +1523,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" ht="17">
+    <row r="10" spans="1:22" ht="16.5">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1543,7 +1556,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" ht="17">
+    <row r="11" spans="1:22" ht="16.5">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1576,7 +1589,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" ht="17">
+    <row r="12" spans="1:22" ht="16.5">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1609,7 +1622,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" ht="17">
+    <row r="13" spans="1:22" ht="16.5">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1642,7 +1655,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" ht="17">
+    <row r="14" spans="1:22" ht="16.5">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1919,9 +1932,9 @@
       <selection activeCell="K23" sqref="A18:K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="17">
+    <row r="1" spans="1:11" ht="16.5">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>18</v>
@@ -1954,7 +1967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17">
+    <row r="2" spans="1:11" ht="16.5">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1985,7 +1998,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" ht="17">
+    <row r="3" spans="1:11" ht="16.5">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -2016,7 +2029,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="17">
+    <row r="4" spans="1:11" ht="16.5">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -2047,7 +2060,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="17">
+    <row r="5" spans="1:11" ht="16.5">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -2078,7 +2091,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" ht="17">
+    <row r="6" spans="1:11" ht="16.5">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -2109,7 +2122,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" ht="17">
+    <row r="7" spans="1:11" ht="16.5">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -2140,7 +2153,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:11" ht="17">
+    <row r="8" spans="1:11" ht="16.5">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -2171,7 +2184,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" spans="1:11" ht="17">
+    <row r="9" spans="1:11" ht="16.5">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -2202,7 +2215,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" ht="17">
+    <row r="10" spans="1:11" ht="16.5">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -2233,7 +2246,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" ht="17">
+    <row r="11" spans="1:11" ht="16.5">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -2264,7 +2277,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" ht="17">
+    <row r="12" spans="1:11" ht="16.5">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -2295,7 +2308,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" ht="17">
+    <row r="13" spans="1:11" ht="16.5">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -2326,7 +2339,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="17">
+    <row r="14" spans="1:11" ht="16.5">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -2357,7 +2370,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" ht="17">
+    <row r="15" spans="1:11" ht="16.5">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -2388,7 +2401,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" ht="17">
+    <row r="16" spans="1:11" ht="16.5">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -2419,7 +2432,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:11" ht="17">
+    <row r="17" spans="1:11" ht="16.5">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -2667,9 +2680,9 @@
       <selection activeCell="H11" sqref="A7:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="17">
+    <row r="1" spans="1:9" ht="16.5">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>8</v>
@@ -2696,7 +2709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17">
+    <row r="2" spans="1:9" ht="16.5">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -2721,7 +2734,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:9" ht="16.5">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -2746,7 +2759,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" ht="17">
+    <row r="4" spans="1:9" ht="16.5">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -2771,7 +2784,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="17">
+    <row r="5" spans="1:9" ht="16.5">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -2796,7 +2809,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="17">
+    <row r="6" spans="1:9" ht="16.5">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -2894,9 +2907,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24">
+    <row r="1" spans="1:9" ht="21">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -2923,7 +2936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17">
+    <row r="2" spans="1:9" ht="16.5">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2948,7 +2961,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:9" ht="16.5">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -2973,7 +2986,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="17">
+    <row r="4" spans="1:9" ht="16.5">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -2998,7 +3011,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="17">
+    <row r="5" spans="1:9" ht="16.5">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -3023,7 +3036,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="17">
+    <row r="6" spans="1:9" ht="16.5">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -3048,7 +3061,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="17">
+    <row r="7" spans="1:9" ht="16.5">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -3126,9 +3139,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3349,27 +3365,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3394,9 +3398,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>